<commit_message>
MTL env setup. Keywords and Programs to be filled
</commit_message>
<xml_diff>
--- a/database/MaterialsScience/MTL_Course_database.xlsx
+++ b/database/MaterialsScience/MTL_Course_database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\Materials_Science\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\MaterialsScience\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182F491B-F54E-4FAA-838F-81D6F9E2530D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EFC89C-303A-4E29-AA81-A95D790556F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="-14655" windowWidth="17115" windowHeight="13605" xr2:uid="{4A678F9F-A21C-41A5-9AEE-FA5C928DC178}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4A678F9F-A21C-41A5-9AEE-FA5C928DC178}"/>
   </bookViews>
   <sheets>
     <sheet name="All_MTL_Courses" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>普通物理學(一)</t>
   </si>
@@ -34,12 +34,6 @@
   </si>
   <si>
     <t>微積分(一)</t>
-  </si>
-  <si>
-    <t>數位邏輯</t>
-  </si>
-  <si>
-    <t>嵌入式程式設計</t>
   </si>
   <si>
     <t>電路學(一)</t>
@@ -52,9 +46,6 @@
   </si>
   <si>
     <t>離散數學</t>
-  </si>
-  <si>
-    <t>電子學(三)</t>
   </si>
   <si>
     <t>近代物理</t>
@@ -111,18 +102,6 @@
     <t>電子元件與材料</t>
   </si>
   <si>
-    <t>聲學</t>
-  </si>
-  <si>
-    <t>微系統製造</t>
-  </si>
-  <si>
-    <t>電動機</t>
-  </si>
-  <si>
-    <t>電力電子實驗</t>
-  </si>
-  <si>
     <t>電子實驗(一)</t>
   </si>
   <si>
@@ -153,88 +132,13 @@
     <t>熱傳學</t>
   </si>
   <si>
-    <t>機動學</t>
-  </si>
-  <si>
     <t>工程材料</t>
-  </si>
-  <si>
-    <t>工程圖學</t>
-  </si>
-  <si>
-    <t>工廠實習</t>
-  </si>
-  <si>
-    <t>機械工程概論</t>
-  </si>
-  <si>
-    <t>測量原理與機工實驗</t>
-  </si>
-  <si>
-    <t>機械工程實務</t>
-  </si>
-  <si>
-    <t>普通化學</t>
-  </si>
-  <si>
-    <t>機械製造</t>
   </si>
   <si>
     <t>基礎程式設計一</t>
   </si>
   <si>
     <t>基礎程式設計二</t>
-  </si>
-  <si>
-    <t>機械繪圖</t>
-  </si>
-  <si>
-    <t>機械振動</t>
-  </si>
-  <si>
-    <t>機械系統分析</t>
-  </si>
-  <si>
-    <t>機電整合</t>
-  </si>
-  <si>
-    <t>電腦輔助分析</t>
-  </si>
-  <si>
-    <t>車輛動力學</t>
-  </si>
-  <si>
-    <t>內燃機</t>
-  </si>
-  <si>
-    <t>汽車工程原理</t>
-  </si>
-  <si>
-    <t>熱機學</t>
-  </si>
-  <si>
-    <t>汽車設計</t>
-  </si>
-  <si>
-    <t>自動變速</t>
-  </si>
-  <si>
-    <t>車輛控制系統</t>
-  </si>
-  <si>
-    <t>懸吊系統</t>
-  </si>
-  <si>
-    <t>機構設計</t>
-  </si>
-  <si>
-    <t>機械設計原理</t>
-  </si>
-  <si>
-    <t>機械設計</t>
-  </si>
-  <si>
-    <t>機械製圖</t>
   </si>
   <si>
     <t>熱力學一</t>
@@ -255,12 +159,6 @@
     <t>材料力學一</t>
   </si>
   <si>
-    <t>機構學</t>
-  </si>
-  <si>
-    <t>自動化科技</t>
-  </si>
-  <si>
     <t>醫學工程材料</t>
   </si>
   <si>
@@ -270,22 +168,7 @@
     <t>流體力學二</t>
   </si>
   <si>
-    <t>航太工程概論</t>
-  </si>
-  <si>
-    <t>微機電系統理論</t>
-  </si>
-  <si>
-    <t>風力發電</t>
-  </si>
-  <si>
-    <t>電力電子學</t>
-  </si>
-  <si>
     <t>熱處理技術</t>
-  </si>
-  <si>
-    <t>再生能源系統</t>
   </si>
   <si>
     <t>機械過程預處理</t>
@@ -294,13 +177,7 @@
     <t>材料結構與物性</t>
   </si>
   <si>
-    <t>材料性質</t>
-  </si>
-  <si>
     <t>動態系統分析</t>
-  </si>
-  <si>
-    <t>電驅動</t>
   </si>
   <si>
     <t>材料流動與物流</t>
@@ -309,28 +186,67 @@
     <t>輕質結構</t>
   </si>
   <si>
-    <t>機械加工</t>
-  </si>
-  <si>
     <t>物流管理</t>
-  </si>
-  <si>
-    <t>實驗規劃與統計</t>
-  </si>
-  <si>
-    <t>渦輪機構</t>
-  </si>
-  <si>
-    <t>航空發動機</t>
-  </si>
-  <si>
-    <t>振動聲學</t>
   </si>
   <si>
     <t>塑料工程</t>
   </si>
   <si>
     <t>能源系統</t>
+  </si>
+  <si>
+    <t>普通化學(一)</t>
+  </si>
+  <si>
+    <t>普通化學(二)</t>
+  </si>
+  <si>
+    <t>應用力學</t>
+  </si>
+  <si>
+    <t>材料熱力學</t>
+  </si>
+  <si>
+    <t>有機化學</t>
+  </si>
+  <si>
+    <t>材料物理性質</t>
+  </si>
+  <si>
+    <t>高分子導論</t>
+  </si>
+  <si>
+    <t>結晶與繞射導論</t>
+  </si>
+  <si>
+    <t>材料實驗(一)</t>
+  </si>
+  <si>
+    <t>材料實驗(二)</t>
+  </si>
+  <si>
+    <t>高分子化學</t>
+  </si>
+  <si>
+    <t>高分子物理</t>
+  </si>
+  <si>
+    <t>高分子加工</t>
+  </si>
+  <si>
+    <t>材料分析</t>
+  </si>
+  <si>
+    <t>半導體材料物理</t>
+  </si>
+  <si>
+    <t>固態物理</t>
+  </si>
+  <si>
+    <t>奈米材料導論</t>
+  </si>
+  <si>
+    <t>材料結構與缺陷</t>
   </si>
 </sst>
 </file>
@@ -415,7 +331,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -447,7 +363,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -763,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C323114-BC5F-49C1-9F53-9EA9AB7CC060}">
-  <dimension ref="A1:W424"/>
+  <dimension ref="A1:W426"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -777,7 +692,7 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -827,7 +742,7 @@
     </row>
     <row r="3" spans="1:23">
       <c r="A3" s="9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -852,7 +767,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -877,7 +792,7 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="9" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -902,7 +817,7 @@
     </row>
     <row r="6" spans="1:23">
       <c r="A6" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -927,7 +842,7 @@
     </row>
     <row r="7" spans="1:23">
       <c r="A7" s="9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" s="5"/>
       <c r="D7" s="5"/>
@@ -951,7 +866,7 @@
     </row>
     <row r="8" spans="1:23">
       <c r="A8" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B8" s="5"/>
       <c r="D8" s="5"/>
@@ -975,7 +890,7 @@
     </row>
     <row r="9" spans="1:23">
       <c r="A9" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B9" s="5"/>
       <c r="D9" s="5"/>
@@ -1023,7 +938,7 @@
     </row>
     <row r="11" spans="1:23">
       <c r="A11" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B11" s="5"/>
       <c r="D11" s="5"/>
@@ -1071,7 +986,7 @@
     </row>
     <row r="13" spans="1:23">
       <c r="A13" s="9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B13" s="5"/>
       <c r="D13" s="5"/>
@@ -1095,7 +1010,7 @@
     </row>
     <row r="14" spans="1:23">
       <c r="A14" s="9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B14" s="5"/>
       <c r="D14" s="5"/>
@@ -1119,7 +1034,7 @@
     </row>
     <row r="15" spans="1:23">
       <c r="A15" s="9" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="B15" s="5"/>
       <c r="D15" s="5"/>
@@ -1142,8 +1057,8 @@
       <c r="W15" s="7"/>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="10" t="s">
-        <v>51</v>
+      <c r="A16" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="B16" s="5"/>
       <c r="D16" s="5"/>
@@ -1166,8 +1081,8 @@
       <c r="W16" s="7"/>
     </row>
     <row r="17" spans="1:23">
-      <c r="A17" s="10" t="s">
-        <v>52</v>
+      <c r="A17" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="B17" s="5"/>
       <c r="D17" s="5"/>
@@ -1190,8 +1105,8 @@
       <c r="W17" s="7"/>
     </row>
     <row r="18" spans="1:23">
-      <c r="A18" s="11" t="s">
-        <v>53</v>
+      <c r="A18" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="B18" s="5"/>
       <c r="D18" s="5"/>
@@ -1214,8 +1129,8 @@
       <c r="W18" s="7"/>
     </row>
     <row r="19" spans="1:23">
-      <c r="A19" s="9" t="s">
-        <v>4</v>
+      <c r="A19" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="B19" s="5"/>
       <c r="D19" s="5"/>
@@ -1238,8 +1153,8 @@
       <c r="W19" s="7"/>
     </row>
     <row r="20" spans="1:23">
-      <c r="A20" s="9" t="s">
-        <v>37</v>
+      <c r="A20" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="B20" s="5"/>
       <c r="D20" s="5"/>
@@ -1258,12 +1173,12 @@
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
       <c r="U20" s="5"/>
-      <c r="V20" s="5"/>
+      <c r="V20" s="1"/>
       <c r="W20" s="7"/>
     </row>
     <row r="21" spans="1:23">
       <c r="A21" s="9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B21" s="5"/>
       <c r="D21" s="5"/>
@@ -1282,12 +1197,12 @@
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
-      <c r="V21" s="5"/>
+      <c r="V21" s="1"/>
       <c r="W21" s="7"/>
     </row>
     <row r="22" spans="1:23">
-      <c r="A22" s="9" t="s">
-        <v>24</v>
+      <c r="A22" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="B22" s="5"/>
       <c r="D22" s="5"/>
@@ -1310,8 +1225,8 @@
       <c r="W22" s="7"/>
     </row>
     <row r="23" spans="1:23">
-      <c r="A23" s="9" t="s">
-        <v>26</v>
+      <c r="A23" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="B23" s="5"/>
       <c r="D23" s="5"/>
@@ -1335,7 +1250,7 @@
     </row>
     <row r="24" spans="1:23">
       <c r="A24" s="9" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="B24" s="5"/>
       <c r="D24" s="5"/>
@@ -1354,12 +1269,12 @@
       <c r="S24" s="5"/>
       <c r="T24" s="5"/>
       <c r="U24" s="5"/>
-      <c r="V24" s="1"/>
+      <c r="V24" s="5"/>
       <c r="W24" s="7"/>
     </row>
     <row r="25" spans="1:23">
       <c r="A25" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" s="5"/>
       <c r="D25" s="5"/>
@@ -1378,12 +1293,12 @@
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
       <c r="U25" s="5"/>
-      <c r="V25" s="1"/>
+      <c r="V25" s="5"/>
       <c r="W25" s="7"/>
     </row>
     <row r="26" spans="1:23">
-      <c r="A26" s="10" t="s">
-        <v>25</v>
+      <c r="A26" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="B26" s="5"/>
       <c r="D26" s="5"/>
@@ -1407,7 +1322,7 @@
     </row>
     <row r="27" spans="1:23">
       <c r="A27" s="9" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B27" s="5"/>
       <c r="D27" s="5"/>
@@ -1431,7 +1346,7 @@
     </row>
     <row r="28" spans="1:23">
       <c r="A28" s="9" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B28" s="5"/>
       <c r="D28" s="5"/>
@@ -1455,7 +1370,7 @@
     </row>
     <row r="29" spans="1:23">
       <c r="A29" s="9" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B29" s="5"/>
       <c r="D29" s="5"/>
@@ -1478,8 +1393,8 @@
       <c r="W29" s="7"/>
     </row>
     <row r="30" spans="1:23">
-      <c r="A30" s="9" t="s">
-        <v>14</v>
+      <c r="A30" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="B30" s="5"/>
       <c r="D30" s="5"/>
@@ -1502,8 +1417,8 @@
       <c r="W30" s="7"/>
     </row>
     <row r="31" spans="1:23">
-      <c r="A31" s="9" t="s">
-        <v>9</v>
+      <c r="A31" s="11" t="s">
+        <v>70</v>
       </c>
       <c r="B31" s="5"/>
       <c r="D31" s="5"/>
@@ -1527,7 +1442,7 @@
     </row>
     <row r="32" spans="1:23">
       <c r="A32" s="9" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B32" s="5"/>
       <c r="D32" s="5"/>
@@ -1551,7 +1466,7 @@
     </row>
     <row r="33" spans="1:23">
       <c r="A33" s="9" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B33" s="5"/>
       <c r="D33" s="5"/>
@@ -1570,12 +1485,12 @@
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
       <c r="U33" s="5"/>
-      <c r="V33" s="5"/>
+      <c r="V33" s="1"/>
       <c r="W33" s="7"/>
     </row>
     <row r="34" spans="1:23">
       <c r="A34" s="9" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B34" s="5"/>
       <c r="D34" s="5"/>
@@ -1594,12 +1509,12 @@
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
       <c r="U34" s="5"/>
-      <c r="V34" s="5"/>
+      <c r="V34" s="1"/>
       <c r="W34" s="7"/>
     </row>
     <row r="35" spans="1:23">
       <c r="A35" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B35" s="5"/>
       <c r="D35" s="5"/>
@@ -1618,12 +1533,12 @@
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
       <c r="U35" s="5"/>
-      <c r="V35" s="5"/>
+      <c r="V35" s="1"/>
       <c r="W35" s="7"/>
     </row>
     <row r="36" spans="1:23">
       <c r="A36" s="9" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B36" s="5"/>
       <c r="D36" s="5"/>
@@ -1647,7 +1562,7 @@
     </row>
     <row r="37" spans="1:23">
       <c r="A37" s="9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B37" s="5"/>
       <c r="D37" s="5"/>
@@ -1671,7 +1586,7 @@
     </row>
     <row r="38" spans="1:23">
       <c r="A38" s="9" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B38" s="5"/>
       <c r="D38" s="5"/>
@@ -1695,7 +1610,7 @@
     </row>
     <row r="39" spans="1:23">
       <c r="A39" s="9" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="B39" s="5"/>
       <c r="D39" s="5"/>
@@ -1714,12 +1629,12 @@
       <c r="S39" s="5"/>
       <c r="T39" s="5"/>
       <c r="U39" s="5"/>
-      <c r="V39" s="1"/>
+      <c r="V39" s="5"/>
       <c r="W39" s="7"/>
     </row>
     <row r="40" spans="1:23">
-      <c r="A40" s="11" t="s">
-        <v>39</v>
+      <c r="A40" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="B40" s="5"/>
       <c r="D40" s="5"/>
@@ -1738,12 +1653,12 @@
       <c r="S40" s="5"/>
       <c r="T40" s="5"/>
       <c r="U40" s="5"/>
-      <c r="V40" s="1"/>
+      <c r="V40" s="5"/>
       <c r="W40" s="7"/>
     </row>
     <row r="41" spans="1:23">
-      <c r="A41" s="12" t="s">
-        <v>40</v>
+      <c r="A41" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="B41" s="5"/>
       <c r="D41" s="5"/>
@@ -1762,12 +1677,12 @@
       <c r="S41" s="5"/>
       <c r="T41" s="5"/>
       <c r="U41" s="5"/>
-      <c r="V41" s="1"/>
+      <c r="V41" s="5"/>
       <c r="W41" s="7"/>
     </row>
     <row r="42" spans="1:23">
-      <c r="A42" s="12" t="s">
-        <v>70</v>
+      <c r="A42" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="B42" s="5"/>
       <c r="D42" s="5"/>
@@ -1790,8 +1705,8 @@
       <c r="W42" s="7"/>
     </row>
     <row r="43" spans="1:23">
-      <c r="A43" s="12" t="s">
-        <v>71</v>
+      <c r="A43" s="11" t="s">
+        <v>32</v>
       </c>
       <c r="B43" s="5"/>
       <c r="D43" s="5"/>
@@ -1815,7 +1730,7 @@
     </row>
     <row r="44" spans="1:23">
       <c r="A44" s="12" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="B44" s="5"/>
       <c r="D44" s="5"/>
@@ -1839,7 +1754,7 @@
     </row>
     <row r="45" spans="1:23">
       <c r="A45" s="12" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B45" s="5"/>
       <c r="D45" s="5"/>
@@ -1863,7 +1778,7 @@
     </row>
     <row r="46" spans="1:23">
       <c r="A46" s="12" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="B46" s="5"/>
       <c r="D46" s="5"/>
@@ -1887,7 +1802,7 @@
     </row>
     <row r="47" spans="1:23">
       <c r="A47" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B47" s="5"/>
       <c r="D47" s="5"/>
@@ -1911,7 +1826,7 @@
     </row>
     <row r="48" spans="1:23">
       <c r="A48" s="12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B48" s="5"/>
       <c r="D48" s="5"/>
@@ -1935,7 +1850,7 @@
     </row>
     <row r="49" spans="1:23">
       <c r="A49" s="12" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B49" s="5"/>
       <c r="D49" s="5"/>
@@ -1959,7 +1874,7 @@
     </row>
     <row r="50" spans="1:23">
       <c r="A50" s="12" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B50" s="5"/>
       <c r="D50" s="5"/>
@@ -1983,7 +1898,7 @@
     </row>
     <row r="51" spans="1:23">
       <c r="A51" s="12" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B51" s="5"/>
       <c r="D51" s="5"/>
@@ -2007,7 +1922,7 @@
     </row>
     <row r="52" spans="1:23">
       <c r="A52" s="12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B52" s="5"/>
       <c r="D52" s="5"/>
@@ -2031,7 +1946,7 @@
     </row>
     <row r="53" spans="1:23">
       <c r="A53" s="12" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="B53" s="5"/>
       <c r="D53" s="5"/>
@@ -2055,7 +1970,7 @@
     </row>
     <row r="54" spans="1:23">
       <c r="A54" s="12" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="B54" s="5"/>
       <c r="D54" s="5"/>
@@ -2079,7 +1994,7 @@
     </row>
     <row r="55" spans="1:23">
       <c r="A55" s="12" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B55" s="5"/>
       <c r="D55" s="5"/>
@@ -2103,7 +2018,7 @@
     </row>
     <row r="56" spans="1:23">
       <c r="A56" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B56" s="5"/>
       <c r="D56" s="5"/>
@@ -2127,7 +2042,7 @@
     </row>
     <row r="57" spans="1:23">
       <c r="A57" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B57" s="5"/>
       <c r="D57" s="5"/>
@@ -2151,7 +2066,7 @@
     </row>
     <row r="58" spans="1:23">
       <c r="A58" s="12" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B58" s="5"/>
       <c r="D58" s="5"/>
@@ -2175,7 +2090,7 @@
     </row>
     <row r="59" spans="1:23">
       <c r="A59" s="12" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B59" s="5"/>
       <c r="D59" s="5"/>
@@ -2199,7 +2114,7 @@
     </row>
     <row r="60" spans="1:23">
       <c r="A60" s="12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B60" s="5"/>
       <c r="D60" s="5"/>
@@ -2222,8 +2137,8 @@
       <c r="W60" s="7"/>
     </row>
     <row r="61" spans="1:23">
-      <c r="A61" s="13" t="s">
-        <v>67</v>
+      <c r="A61" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="B61" s="5"/>
       <c r="D61" s="5"/>
@@ -2247,7 +2162,7 @@
     </row>
     <row r="62" spans="1:23">
       <c r="A62" s="12" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="B62" s="5"/>
       <c r="D62" s="5"/>
@@ -2271,7 +2186,7 @@
     </row>
     <row r="63" spans="1:23">
       <c r="A63" s="12" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="B63" s="5"/>
       <c r="D63" s="5"/>
@@ -2295,7 +2210,7 @@
     </row>
     <row r="64" spans="1:23">
       <c r="A64" s="12" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="B64" s="5"/>
       <c r="D64" s="5"/>
@@ -2319,7 +2234,7 @@
     </row>
     <row r="65" spans="1:23">
       <c r="A65" s="12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B65" s="5"/>
       <c r="D65" s="5"/>
@@ -2343,7 +2258,7 @@
     </row>
     <row r="66" spans="1:23">
       <c r="A66" s="12" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="B66" s="5"/>
       <c r="D66" s="5"/>
@@ -2367,7 +2282,7 @@
     </row>
     <row r="67" spans="1:23">
       <c r="A67" s="12" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="B67" s="5"/>
       <c r="D67" s="5"/>
@@ -2391,7 +2306,7 @@
     </row>
     <row r="68" spans="1:23">
       <c r="A68" s="12" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="B68" s="5"/>
       <c r="D68" s="5"/>
@@ -2415,7 +2330,7 @@
     </row>
     <row r="69" spans="1:23">
       <c r="A69" s="12" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="B69" s="5"/>
       <c r="D69" s="5"/>
@@ -2439,7 +2354,7 @@
     </row>
     <row r="70" spans="1:23">
       <c r="A70" s="12" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B70" s="5"/>
       <c r="D70" s="5"/>
@@ -2463,7 +2378,7 @@
     </row>
     <row r="71" spans="1:23">
       <c r="A71" s="12" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B71" s="5"/>
       <c r="D71" s="5"/>
@@ -2487,7 +2402,7 @@
     </row>
     <row r="72" spans="1:23">
       <c r="A72" s="12" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B72" s="5"/>
       <c r="D72" s="5"/>
@@ -2511,7 +2426,7 @@
     </row>
     <row r="73" spans="1:23">
       <c r="A73" s="12" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B73" s="5"/>
       <c r="D73" s="5"/>
@@ -2535,7 +2450,7 @@
     </row>
     <row r="74" spans="1:23">
       <c r="A74" s="12" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B74" s="5"/>
       <c r="D74" s="5"/>
@@ -2554,13 +2469,10 @@
       <c r="S74" s="5"/>
       <c r="T74" s="5"/>
       <c r="U74" s="5"/>
-      <c r="V74" s="1"/>
+      <c r="V74" s="5"/>
       <c r="W74" s="7"/>
     </row>
     <row r="75" spans="1:23">
-      <c r="A75" s="12" t="s">
-        <v>59</v>
-      </c>
       <c r="B75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
@@ -2578,13 +2490,10 @@
       <c r="S75" s="5"/>
       <c r="T75" s="5"/>
       <c r="U75" s="5"/>
-      <c r="V75" s="1"/>
+      <c r="V75" s="5"/>
       <c r="W75" s="7"/>
     </row>
     <row r="76" spans="1:23">
-      <c r="A76" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="B76" s="5"/>
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
@@ -2606,9 +2515,6 @@
       <c r="W76" s="7"/>
     </row>
     <row r="77" spans="1:23">
-      <c r="A77" s="12" t="s">
-        <v>61</v>
-      </c>
       <c r="B77" s="5"/>
       <c r="D77" s="5"/>
       <c r="E77" s="5"/>
@@ -2630,9 +2536,6 @@
       <c r="W77" s="7"/>
     </row>
     <row r="78" spans="1:23">
-      <c r="A78" s="12" t="s">
-        <v>62</v>
-      </c>
       <c r="B78" s="5"/>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
@@ -2650,13 +2553,10 @@
       <c r="S78" s="5"/>
       <c r="T78" s="5"/>
       <c r="U78" s="5"/>
-      <c r="V78" s="5"/>
+      <c r="V78" s="1"/>
       <c r="W78" s="7"/>
     </row>
     <row r="79" spans="1:23">
-      <c r="A79" s="12" t="s">
-        <v>63</v>
-      </c>
       <c r="B79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
@@ -2674,13 +2574,10 @@
       <c r="S79" s="5"/>
       <c r="T79" s="5"/>
       <c r="U79" s="5"/>
-      <c r="V79" s="5"/>
+      <c r="V79" s="1"/>
       <c r="W79" s="7"/>
     </row>
     <row r="80" spans="1:23">
-      <c r="A80" s="12" t="s">
-        <v>64</v>
-      </c>
       <c r="B80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="5"/>
@@ -2698,13 +2595,10 @@
       <c r="S80" s="5"/>
       <c r="T80" s="5"/>
       <c r="U80" s="5"/>
-      <c r="V80" s="1"/>
+      <c r="V80" s="5"/>
       <c r="W80" s="7"/>
     </row>
-    <row r="81" spans="1:23">
-      <c r="A81" s="12" t="s">
-        <v>65</v>
-      </c>
+    <row r="81" spans="2:23">
       <c r="B81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
@@ -2722,13 +2616,10 @@
       <c r="S81" s="5"/>
       <c r="T81" s="5"/>
       <c r="U81" s="5"/>
-      <c r="V81" s="1"/>
+      <c r="V81" s="5"/>
       <c r="W81" s="7"/>
     </row>
-    <row r="82" spans="1:23">
-      <c r="A82" s="12" t="s">
-        <v>76</v>
-      </c>
+    <row r="82" spans="2:23">
       <c r="B82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
@@ -2749,10 +2640,7 @@
       <c r="V82" s="1"/>
       <c r="W82" s="7"/>
     </row>
-    <row r="83" spans="1:23">
-      <c r="A83" s="12" t="s">
-        <v>66</v>
-      </c>
+    <row r="83" spans="2:23">
       <c r="B83" s="5"/>
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
@@ -2773,10 +2661,7 @@
       <c r="V83" s="1"/>
       <c r="W83" s="7"/>
     </row>
-    <row r="84" spans="1:23">
-      <c r="A84" s="12" t="s">
-        <v>68</v>
-      </c>
+    <row r="84" spans="2:23">
       <c r="B84" s="5"/>
       <c r="D84" s="5"/>
       <c r="E84" s="5"/>
@@ -2797,10 +2682,7 @@
       <c r="V84" s="1"/>
       <c r="W84" s="7"/>
     </row>
-    <row r="85" spans="1:23">
-      <c r="A85" s="12" t="s">
-        <v>69</v>
-      </c>
+    <row r="85" spans="2:23">
       <c r="B85" s="5"/>
       <c r="D85" s="5"/>
       <c r="E85" s="5"/>
@@ -2818,13 +2700,10 @@
       <c r="S85" s="5"/>
       <c r="T85" s="5"/>
       <c r="U85" s="5"/>
-      <c r="V85" s="5"/>
+      <c r="V85" s="1"/>
       <c r="W85" s="7"/>
     </row>
-    <row r="86" spans="1:23">
-      <c r="A86" s="12" t="s">
-        <v>77</v>
-      </c>
+    <row r="86" spans="2:23">
       <c r="B86" s="5"/>
       <c r="D86" s="5"/>
       <c r="E86" s="5"/>
@@ -2842,13 +2721,10 @@
       <c r="S86" s="5"/>
       <c r="T86" s="5"/>
       <c r="U86" s="5"/>
-      <c r="V86" s="5"/>
+      <c r="V86" s="1"/>
       <c r="W86" s="7"/>
     </row>
-    <row r="87" spans="1:23">
-      <c r="A87" s="12" t="s">
-        <v>78</v>
-      </c>
+    <row r="87" spans="2:23">
       <c r="B87" s="5"/>
       <c r="D87" s="5"/>
       <c r="E87" s="5"/>
@@ -2869,10 +2745,7 @@
       <c r="V87" s="5"/>
       <c r="W87" s="7"/>
     </row>
-    <row r="88" spans="1:23">
-      <c r="A88" s="12" t="s">
-        <v>81</v>
-      </c>
+    <row r="88" spans="2:23">
       <c r="B88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="5"/>
@@ -2893,10 +2766,7 @@
       <c r="V88" s="5"/>
       <c r="W88" s="7"/>
     </row>
-    <row r="89" spans="1:23">
-      <c r="A89" s="12" t="s">
-        <v>82</v>
-      </c>
+    <row r="89" spans="2:23">
       <c r="B89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
@@ -2917,10 +2787,7 @@
       <c r="V89" s="5"/>
       <c r="W89" s="7"/>
     </row>
-    <row r="90" spans="1:23">
-      <c r="A90" s="12" t="s">
-        <v>83</v>
-      </c>
+    <row r="90" spans="2:23">
       <c r="B90" s="5"/>
       <c r="D90" s="5"/>
       <c r="E90" s="5"/>
@@ -2941,10 +2808,7 @@
       <c r="V90" s="5"/>
       <c r="W90" s="7"/>
     </row>
-    <row r="91" spans="1:23">
-      <c r="A91" s="12" t="s">
-        <v>87</v>
-      </c>
+    <row r="91" spans="2:23">
       <c r="B91" s="5"/>
       <c r="D91" s="5"/>
       <c r="E91" s="5"/>
@@ -2965,10 +2829,7 @@
       <c r="V91" s="5"/>
       <c r="W91" s="7"/>
     </row>
-    <row r="92" spans="1:23">
-      <c r="A92" s="12" t="s">
-        <v>91</v>
-      </c>
+    <row r="92" spans="2:23">
       <c r="B92" s="5"/>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
@@ -2989,10 +2850,7 @@
       <c r="V92" s="5"/>
       <c r="W92" s="7"/>
     </row>
-    <row r="93" spans="1:23">
-      <c r="A93" s="12" t="s">
-        <v>92</v>
-      </c>
+    <row r="93" spans="2:23">
       <c r="B93" s="5"/>
       <c r="D93" s="5"/>
       <c r="E93" s="5"/>
@@ -3013,10 +2871,7 @@
       <c r="V93" s="5"/>
       <c r="W93" s="7"/>
     </row>
-    <row r="94" spans="1:23">
-      <c r="A94" s="12" t="s">
-        <v>93</v>
-      </c>
+    <row r="94" spans="2:23">
       <c r="B94" s="5"/>
       <c r="D94" s="5"/>
       <c r="E94" s="5"/>
@@ -3037,10 +2892,7 @@
       <c r="V94" s="5"/>
       <c r="W94" s="7"/>
     </row>
-    <row r="95" spans="1:23">
-      <c r="A95" s="12" t="s">
-        <v>94</v>
-      </c>
+    <row r="95" spans="2:23">
       <c r="B95" s="5"/>
       <c r="D95" s="5"/>
       <c r="E95" s="5"/>
@@ -3061,12 +2913,8 @@
       <c r="V95" s="5"/>
       <c r="W95" s="7"/>
     </row>
-    <row r="96" spans="1:23">
-      <c r="A96" s="12" t="s">
-        <v>95</v>
-      </c>
+    <row r="96" spans="2:23">
       <c r="B96" s="5"/>
-      <c r="C96" s="5"/>
       <c r="D96" s="5"/>
       <c r="E96" s="5"/>
       <c r="H96" s="5"/>
@@ -3087,11 +2935,7 @@
       <c r="W96" s="7"/>
     </row>
     <row r="97" spans="1:23">
-      <c r="A97" s="12" t="s">
-        <v>96</v>
-      </c>
       <c r="B97" s="5"/>
-      <c r="C97" s="5"/>
       <c r="D97" s="5"/>
       <c r="E97" s="5"/>
       <c r="H97" s="5"/>
@@ -3112,9 +2956,6 @@
       <c r="W97" s="7"/>
     </row>
     <row r="98" spans="1:23">
-      <c r="A98" s="12" t="s">
-        <v>97</v>
-      </c>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
@@ -3137,9 +2978,6 @@
       <c r="W98" s="7"/>
     </row>
     <row r="99" spans="1:23">
-      <c r="A99" s="12" t="s">
-        <v>98</v>
-      </c>
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
@@ -3162,9 +3000,6 @@
       <c r="W99" s="7"/>
     </row>
     <row r="100" spans="1:23">
-      <c r="A100" s="12" t="s">
-        <v>99</v>
-      </c>
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
@@ -3187,9 +3022,6 @@
       <c r="W100" s="7"/>
     </row>
     <row r="101" spans="1:23">
-      <c r="A101" s="12" t="s">
-        <v>100</v>
-      </c>
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
@@ -3208,13 +3040,10 @@
       <c r="S101" s="5"/>
       <c r="T101" s="5"/>
       <c r="U101" s="5"/>
-      <c r="V101" s="1"/>
+      <c r="V101" s="5"/>
       <c r="W101" s="7"/>
     </row>
     <row r="102" spans="1:23">
-      <c r="A102" s="12" t="s">
-        <v>101</v>
-      </c>
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
@@ -3233,11 +3062,10 @@
       <c r="S102" s="5"/>
       <c r="T102" s="5"/>
       <c r="U102" s="5"/>
-      <c r="V102" s="1"/>
+      <c r="V102" s="5"/>
       <c r="W102" s="7"/>
     </row>
     <row r="103" spans="1:23">
-      <c r="A103" s="3"/>
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
@@ -3256,11 +3084,10 @@
       <c r="S103" s="5"/>
       <c r="T103" s="5"/>
       <c r="U103" s="5"/>
-      <c r="V103" s="5"/>
+      <c r="V103" s="1"/>
       <c r="W103" s="7"/>
     </row>
     <row r="104" spans="1:23">
-      <c r="A104" s="3"/>
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
@@ -3279,7 +3106,7 @@
       <c r="S104" s="5"/>
       <c r="T104" s="5"/>
       <c r="U104" s="5"/>
-      <c r="V104" s="5"/>
+      <c r="V104" s="1"/>
       <c r="W104" s="7"/>
     </row>
     <row r="105" spans="1:23">
@@ -3394,7 +3221,7 @@
       <c r="S109" s="5"/>
       <c r="T109" s="5"/>
       <c r="U109" s="5"/>
-      <c r="V109" s="1"/>
+      <c r="V109" s="5"/>
       <c r="W109" s="7"/>
     </row>
     <row r="110" spans="1:23">
@@ -3417,10 +3244,11 @@
       <c r="S110" s="5"/>
       <c r="T110" s="5"/>
       <c r="U110" s="5"/>
-      <c r="V110" s="1"/>
+      <c r="V110" s="5"/>
       <c r="W110" s="7"/>
     </row>
     <row r="111" spans="1:23">
+      <c r="A111" s="3"/>
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
@@ -3439,10 +3267,11 @@
       <c r="S111" s="5"/>
       <c r="T111" s="5"/>
       <c r="U111" s="5"/>
-      <c r="V111" s="5"/>
+      <c r="V111" s="1"/>
       <c r="W111" s="7"/>
     </row>
     <row r="112" spans="1:23">
+      <c r="A112" s="3"/>
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
       <c r="D112" s="5"/>
@@ -3461,7 +3290,7 @@
       <c r="S112" s="5"/>
       <c r="T112" s="5"/>
       <c r="U112" s="5"/>
-      <c r="V112" s="5"/>
+      <c r="V112" s="1"/>
       <c r="W112" s="7"/>
     </row>
     <row r="113" spans="1:23">
@@ -3615,7 +3444,7 @@
       <c r="S119" s="5"/>
       <c r="T119" s="5"/>
       <c r="U119" s="5"/>
-      <c r="V119" s="1"/>
+      <c r="V119" s="5"/>
       <c r="W119" s="7"/>
     </row>
     <row r="120" spans="1:23">
@@ -3637,7 +3466,7 @@
       <c r="S120" s="5"/>
       <c r="T120" s="5"/>
       <c r="U120" s="5"/>
-      <c r="V120" s="1"/>
+      <c r="V120" s="5"/>
       <c r="W120" s="7"/>
     </row>
     <row r="121" spans="1:23">
@@ -3707,7 +3536,6 @@
       <c r="W123" s="7"/>
     </row>
     <row r="124" spans="1:23">
-      <c r="A124" s="3"/>
       <c r="B124" s="5"/>
       <c r="C124" s="5"/>
       <c r="D124" s="5"/>
@@ -3752,6 +3580,7 @@
       <c r="W125" s="7"/>
     </row>
     <row r="126" spans="1:23">
+      <c r="A126" s="3"/>
       <c r="B126" s="5"/>
       <c r="C126" s="5"/>
       <c r="D126" s="5"/>
@@ -3836,7 +3665,7 @@
       <c r="S129" s="5"/>
       <c r="T129" s="5"/>
       <c r="U129" s="5"/>
-      <c r="V129" s="5"/>
+      <c r="V129" s="1"/>
       <c r="W129" s="7"/>
     </row>
     <row r="130" spans="1:23">
@@ -3858,11 +3687,10 @@
       <c r="S130" s="5"/>
       <c r="T130" s="5"/>
       <c r="U130" s="5"/>
-      <c r="V130" s="5"/>
+      <c r="V130" s="1"/>
       <c r="W130" s="7"/>
     </row>
     <row r="131" spans="1:23">
-      <c r="A131" s="3"/>
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
       <c r="D131" s="5"/>
@@ -3881,7 +3709,7 @@
       <c r="S131" s="5"/>
       <c r="T131" s="5"/>
       <c r="U131" s="5"/>
-      <c r="V131" s="1"/>
+      <c r="V131" s="5"/>
       <c r="W131" s="7"/>
     </row>
     <row r="132" spans="1:23">
@@ -3926,7 +3754,7 @@
       <c r="S133" s="5"/>
       <c r="T133" s="5"/>
       <c r="U133" s="5"/>
-      <c r="V133" s="5"/>
+      <c r="V133" s="1"/>
       <c r="W133" s="7"/>
     </row>
     <row r="134" spans="1:23">
@@ -3948,10 +3776,11 @@
       <c r="S134" s="5"/>
       <c r="T134" s="5"/>
       <c r="U134" s="5"/>
-      <c r="V134" s="1"/>
+      <c r="V134" s="5"/>
       <c r="W134" s="7"/>
     </row>
     <row r="135" spans="1:23">
+      <c r="A135" s="3"/>
       <c r="B135" s="5"/>
       <c r="C135" s="5"/>
       <c r="D135" s="5"/>
@@ -3970,7 +3799,7 @@
       <c r="S135" s="5"/>
       <c r="T135" s="5"/>
       <c r="U135" s="5"/>
-      <c r="V135" s="1"/>
+      <c r="V135" s="5"/>
       <c r="W135" s="7"/>
     </row>
     <row r="136" spans="1:23">
@@ -4146,7 +3975,7 @@
       <c r="S143" s="5"/>
       <c r="T143" s="5"/>
       <c r="U143" s="5"/>
-      <c r="V143" s="5"/>
+      <c r="V143" s="1"/>
       <c r="W143" s="7"/>
     </row>
     <row r="144" spans="1:23">
@@ -4168,7 +3997,7 @@
       <c r="S144" s="5"/>
       <c r="T144" s="5"/>
       <c r="U144" s="5"/>
-      <c r="V144" s="5"/>
+      <c r="V144" s="1"/>
       <c r="W144" s="7"/>
     </row>
     <row r="145" spans="2:23">
@@ -4190,7 +4019,7 @@
       <c r="S145" s="5"/>
       <c r="T145" s="5"/>
       <c r="U145" s="5"/>
-      <c r="V145" s="1"/>
+      <c r="V145" s="5"/>
       <c r="W145" s="7"/>
     </row>
     <row r="146" spans="2:23">
@@ -4234,7 +4063,7 @@
       <c r="S147" s="5"/>
       <c r="T147" s="5"/>
       <c r="U147" s="5"/>
-      <c r="V147" s="5"/>
+      <c r="V147" s="1"/>
       <c r="W147" s="7"/>
     </row>
     <row r="148" spans="2:23">
@@ -4278,7 +4107,7 @@
       <c r="S149" s="5"/>
       <c r="T149" s="5"/>
       <c r="U149" s="5"/>
-      <c r="V149" s="1"/>
+      <c r="V149" s="5"/>
       <c r="W149" s="7"/>
     </row>
     <row r="150" spans="2:23">
@@ -4300,7 +4129,7 @@
       <c r="S150" s="5"/>
       <c r="T150" s="5"/>
       <c r="U150" s="5"/>
-      <c r="V150" s="1"/>
+      <c r="V150" s="5"/>
       <c r="W150" s="7"/>
     </row>
     <row r="151" spans="2:23">
@@ -4322,7 +4151,7 @@
       <c r="S151" s="5"/>
       <c r="T151" s="5"/>
       <c r="U151" s="5"/>
-      <c r="V151" s="5"/>
+      <c r="V151" s="1"/>
       <c r="W151" s="7"/>
     </row>
     <row r="152" spans="2:23">
@@ -4344,7 +4173,7 @@
       <c r="S152" s="5"/>
       <c r="T152" s="5"/>
       <c r="U152" s="5"/>
-      <c r="V152" s="5"/>
+      <c r="V152" s="1"/>
       <c r="W152" s="7"/>
     </row>
     <row r="153" spans="2:23">
@@ -4674,7 +4503,7 @@
       <c r="S167" s="5"/>
       <c r="T167" s="5"/>
       <c r="U167" s="5"/>
-      <c r="V167" s="1"/>
+      <c r="V167" s="5"/>
       <c r="W167" s="7"/>
     </row>
     <row r="168" spans="2:23">
@@ -4696,7 +4525,7 @@
       <c r="S168" s="5"/>
       <c r="T168" s="5"/>
       <c r="U168" s="5"/>
-      <c r="V168" s="1"/>
+      <c r="V168" s="5"/>
       <c r="W168" s="7"/>
     </row>
     <row r="169" spans="2:23">
@@ -4718,7 +4547,7 @@
       <c r="S169" s="5"/>
       <c r="T169" s="5"/>
       <c r="U169" s="5"/>
-      <c r="V169" s="5"/>
+      <c r="V169" s="1"/>
       <c r="W169" s="7"/>
     </row>
     <row r="170" spans="2:23">
@@ -4740,7 +4569,7 @@
       <c r="S170" s="5"/>
       <c r="T170" s="5"/>
       <c r="U170" s="5"/>
-      <c r="V170" s="5"/>
+      <c r="V170" s="1"/>
       <c r="W170" s="7"/>
     </row>
     <row r="171" spans="2:23">
@@ -4762,7 +4591,7 @@
       <c r="S171" s="5"/>
       <c r="T171" s="5"/>
       <c r="U171" s="5"/>
-      <c r="V171" s="1"/>
+      <c r="V171" s="5"/>
       <c r="W171" s="7"/>
     </row>
     <row r="172" spans="2:23">
@@ -4784,7 +4613,7 @@
       <c r="S172" s="5"/>
       <c r="T172" s="5"/>
       <c r="U172" s="5"/>
-      <c r="V172" s="1"/>
+      <c r="V172" s="5"/>
       <c r="W172" s="7"/>
     </row>
     <row r="173" spans="2:23">
@@ -4806,7 +4635,7 @@
       <c r="S173" s="5"/>
       <c r="T173" s="5"/>
       <c r="U173" s="5"/>
-      <c r="V173" s="5"/>
+      <c r="V173" s="1"/>
       <c r="W173" s="7"/>
     </row>
     <row r="174" spans="2:23">
@@ -4828,7 +4657,7 @@
       <c r="S174" s="5"/>
       <c r="T174" s="5"/>
       <c r="U174" s="5"/>
-      <c r="V174" s="5"/>
+      <c r="V174" s="1"/>
       <c r="W174" s="7"/>
     </row>
     <row r="175" spans="2:23">
@@ -5158,7 +4987,7 @@
       <c r="S189" s="5"/>
       <c r="T189" s="5"/>
       <c r="U189" s="5"/>
-      <c r="V189" s="1"/>
+      <c r="V189" s="5"/>
       <c r="W189" s="7"/>
     </row>
     <row r="190" spans="2:23">
@@ -5180,7 +5009,7 @@
       <c r="S190" s="5"/>
       <c r="T190" s="5"/>
       <c r="U190" s="5"/>
-      <c r="V190" s="1"/>
+      <c r="V190" s="5"/>
       <c r="W190" s="7"/>
     </row>
     <row r="191" spans="2:23">
@@ -5246,7 +5075,7 @@
       <c r="S193" s="5"/>
       <c r="T193" s="5"/>
       <c r="U193" s="5"/>
-      <c r="V193" s="5"/>
+      <c r="V193" s="1"/>
       <c r="W193" s="7"/>
     </row>
     <row r="194" spans="2:23">
@@ -5268,7 +5097,7 @@
       <c r="S194" s="5"/>
       <c r="T194" s="5"/>
       <c r="U194" s="5"/>
-      <c r="V194" s="5"/>
+      <c r="V194" s="1"/>
       <c r="W194" s="7"/>
     </row>
     <row r="195" spans="2:23">
@@ -5334,7 +5163,7 @@
       <c r="S197" s="5"/>
       <c r="T197" s="5"/>
       <c r="U197" s="5"/>
-      <c r="V197" s="1"/>
+      <c r="V197" s="5"/>
       <c r="W197" s="7"/>
     </row>
     <row r="198" spans="2:23">
@@ -5356,7 +5185,7 @@
       <c r="S198" s="5"/>
       <c r="T198" s="5"/>
       <c r="U198" s="5"/>
-      <c r="V198" s="1"/>
+      <c r="V198" s="5"/>
       <c r="W198" s="7"/>
     </row>
     <row r="199" spans="2:23">
@@ -5378,7 +5207,7 @@
       <c r="S199" s="5"/>
       <c r="T199" s="5"/>
       <c r="U199" s="5"/>
-      <c r="V199" s="5"/>
+      <c r="V199" s="1"/>
       <c r="W199" s="7"/>
     </row>
     <row r="200" spans="2:23">
@@ -5400,7 +5229,7 @@
       <c r="S200" s="5"/>
       <c r="T200" s="5"/>
       <c r="U200" s="5"/>
-      <c r="V200" s="5"/>
+      <c r="V200" s="1"/>
       <c r="W200" s="7"/>
     </row>
     <row r="201" spans="2:23">
@@ -5598,7 +5427,7 @@
       <c r="S209" s="5"/>
       <c r="T209" s="5"/>
       <c r="U209" s="5"/>
-      <c r="V209" s="1"/>
+      <c r="V209" s="5"/>
       <c r="W209" s="7"/>
     </row>
     <row r="210" spans="1:23">
@@ -5620,11 +5449,10 @@
       <c r="S210" s="5"/>
       <c r="T210" s="5"/>
       <c r="U210" s="5"/>
-      <c r="V210" s="1"/>
+      <c r="V210" s="5"/>
       <c r="W210" s="7"/>
     </row>
     <row r="211" spans="1:23">
-      <c r="A211" s="3"/>
       <c r="B211" s="5"/>
       <c r="C211" s="5"/>
       <c r="D211" s="5"/>
@@ -5643,7 +5471,7 @@
       <c r="S211" s="5"/>
       <c r="T211" s="5"/>
       <c r="U211" s="5"/>
-      <c r="V211" s="5"/>
+      <c r="V211" s="1"/>
       <c r="W211" s="7"/>
     </row>
     <row r="212" spans="1:23">
@@ -5665,11 +5493,11 @@
       <c r="S212" s="5"/>
       <c r="T212" s="5"/>
       <c r="U212" s="5"/>
-      <c r="V212" s="5"/>
+      <c r="V212" s="1"/>
       <c r="W212" s="7"/>
     </row>
     <row r="213" spans="1:23">
-      <c r="A213" s="8"/>
+      <c r="A213" s="3"/>
       <c r="B213" s="5"/>
       <c r="C213" s="5"/>
       <c r="D213" s="5"/>
@@ -5692,7 +5520,6 @@
       <c r="W213" s="7"/>
     </row>
     <row r="214" spans="1:23">
-      <c r="A214" s="3"/>
       <c r="B214" s="5"/>
       <c r="C214" s="5"/>
       <c r="D214" s="5"/>
@@ -5715,7 +5542,7 @@
       <c r="W214" s="7"/>
     </row>
     <row r="215" spans="1:23">
-      <c r="A215" s="3"/>
+      <c r="A215" s="8"/>
       <c r="B215" s="5"/>
       <c r="C215" s="5"/>
       <c r="D215" s="5"/>
@@ -5734,10 +5561,11 @@
       <c r="S215" s="5"/>
       <c r="T215" s="5"/>
       <c r="U215" s="5"/>
-      <c r="V215" s="1"/>
+      <c r="V215" s="5"/>
       <c r="W215" s="7"/>
     </row>
     <row r="216" spans="1:23">
+      <c r="A216" s="3"/>
       <c r="B216" s="5"/>
       <c r="C216" s="5"/>
       <c r="D216" s="5"/>
@@ -5756,10 +5584,11 @@
       <c r="S216" s="5"/>
       <c r="T216" s="5"/>
       <c r="U216" s="5"/>
-      <c r="V216" s="1"/>
+      <c r="V216" s="5"/>
       <c r="W216" s="7"/>
     </row>
     <row r="217" spans="1:23">
+      <c r="A217" s="3"/>
       <c r="B217" s="5"/>
       <c r="C217" s="5"/>
       <c r="D217" s="5"/>
@@ -5778,7 +5607,7 @@
       <c r="S217" s="5"/>
       <c r="T217" s="5"/>
       <c r="U217" s="5"/>
-      <c r="V217" s="5"/>
+      <c r="V217" s="1"/>
       <c r="W217" s="7"/>
     </row>
     <row r="218" spans="1:23">
@@ -5800,7 +5629,7 @@
       <c r="S218" s="5"/>
       <c r="T218" s="5"/>
       <c r="U218" s="5"/>
-      <c r="V218" s="5"/>
+      <c r="V218" s="1"/>
       <c r="W218" s="7"/>
     </row>
     <row r="219" spans="1:23">
@@ -6222,7 +6051,6 @@
       <c r="W237" s="7"/>
     </row>
     <row r="238" spans="1:23">
-      <c r="A238" s="8"/>
       <c r="B238" s="5"/>
       <c r="C238" s="5"/>
       <c r="D238" s="5"/>
@@ -6290,7 +6118,6 @@
       <c r="W240" s="7"/>
     </row>
     <row r="241" spans="1:23">
-      <c r="A241" s="3"/>
       <c r="B241" s="5"/>
       <c r="C241" s="5"/>
       <c r="D241" s="5"/>
@@ -6313,6 +6140,7 @@
       <c r="W241" s="7"/>
     </row>
     <row r="242" spans="1:23">
+      <c r="A242" s="8"/>
       <c r="B242" s="5"/>
       <c r="C242" s="5"/>
       <c r="D242" s="5"/>
@@ -6335,6 +6163,7 @@
       <c r="W242" s="7"/>
     </row>
     <row r="243" spans="1:23">
+      <c r="A243" s="3"/>
       <c r="B243" s="5"/>
       <c r="C243" s="5"/>
       <c r="D243" s="5"/>
@@ -6353,7 +6182,7 @@
       <c r="S243" s="5"/>
       <c r="T243" s="5"/>
       <c r="U243" s="5"/>
-      <c r="V243" s="1"/>
+      <c r="V243" s="5"/>
       <c r="W243" s="7"/>
     </row>
     <row r="244" spans="1:23">
@@ -6375,11 +6204,10 @@
       <c r="S244" s="5"/>
       <c r="T244" s="5"/>
       <c r="U244" s="5"/>
-      <c r="V244" s="1"/>
+      <c r="V244" s="5"/>
       <c r="W244" s="7"/>
     </row>
     <row r="245" spans="1:23">
-      <c r="A245" s="8"/>
       <c r="B245" s="5"/>
       <c r="C245" s="5"/>
       <c r="D245" s="5"/>
@@ -6398,7 +6226,7 @@
       <c r="S245" s="5"/>
       <c r="T245" s="5"/>
       <c r="U245" s="5"/>
-      <c r="V245" s="5"/>
+      <c r="V245" s="1"/>
       <c r="W245" s="7"/>
     </row>
     <row r="246" spans="1:23">
@@ -6420,7 +6248,7 @@
       <c r="S246" s="5"/>
       <c r="T246" s="5"/>
       <c r="U246" s="5"/>
-      <c r="V246" s="5"/>
+      <c r="V246" s="1"/>
       <c r="W246" s="7"/>
     </row>
     <row r="247" spans="1:23">
@@ -6443,7 +6271,7 @@
       <c r="S247" s="5"/>
       <c r="T247" s="5"/>
       <c r="U247" s="5"/>
-      <c r="V247" s="1"/>
+      <c r="V247" s="5"/>
       <c r="W247" s="7"/>
     </row>
     <row r="248" spans="1:23">
@@ -6469,6 +6297,7 @@
       <c r="W248" s="7"/>
     </row>
     <row r="249" spans="1:23">
+      <c r="A249" s="8"/>
       <c r="B249" s="5"/>
       <c r="C249" s="5"/>
       <c r="D249" s="5"/>
@@ -6487,7 +6316,7 @@
       <c r="S249" s="5"/>
       <c r="T249" s="5"/>
       <c r="U249" s="5"/>
-      <c r="V249" s="5"/>
+      <c r="V249" s="1"/>
       <c r="W249" s="7"/>
     </row>
     <row r="250" spans="1:23">
@@ -6509,7 +6338,7 @@
       <c r="S250" s="5"/>
       <c r="T250" s="5"/>
       <c r="U250" s="5"/>
-      <c r="V250" s="1"/>
+      <c r="V250" s="5"/>
       <c r="W250" s="7"/>
     </row>
     <row r="251" spans="1:23">
@@ -6531,7 +6360,7 @@
       <c r="S251" s="5"/>
       <c r="T251" s="5"/>
       <c r="U251" s="5"/>
-      <c r="V251" s="1"/>
+      <c r="V251" s="5"/>
       <c r="W251" s="7"/>
     </row>
     <row r="252" spans="1:23">
@@ -6597,7 +6426,7 @@
       <c r="S254" s="5"/>
       <c r="T254" s="5"/>
       <c r="U254" s="5"/>
-      <c r="V254" s="5"/>
+      <c r="V254" s="1"/>
       <c r="W254" s="7"/>
     </row>
     <row r="255" spans="1:23">
@@ -6619,7 +6448,7 @@
       <c r="S255" s="5"/>
       <c r="T255" s="5"/>
       <c r="U255" s="5"/>
-      <c r="V255" s="5"/>
+      <c r="V255" s="1"/>
       <c r="W255" s="7"/>
     </row>
     <row r="256" spans="1:23">
@@ -6685,7 +6514,7 @@
       <c r="S258" s="5"/>
       <c r="T258" s="5"/>
       <c r="U258" s="5"/>
-      <c r="V258" s="1"/>
+      <c r="V258" s="5"/>
       <c r="W258" s="7"/>
     </row>
     <row r="259" spans="2:23">
@@ -6707,7 +6536,7 @@
       <c r="S259" s="5"/>
       <c r="T259" s="5"/>
       <c r="U259" s="5"/>
-      <c r="V259" s="1"/>
+      <c r="V259" s="5"/>
       <c r="W259" s="7"/>
     </row>
     <row r="260" spans="2:23">
@@ -6729,7 +6558,7 @@
       <c r="S260" s="5"/>
       <c r="T260" s="5"/>
       <c r="U260" s="5"/>
-      <c r="V260" s="5"/>
+      <c r="V260" s="1"/>
       <c r="W260" s="7"/>
     </row>
     <row r="261" spans="2:23">
@@ -6751,7 +6580,7 @@
       <c r="S261" s="5"/>
       <c r="T261" s="5"/>
       <c r="U261" s="5"/>
-      <c r="V261" s="5"/>
+      <c r="V261" s="1"/>
       <c r="W261" s="7"/>
     </row>
     <row r="262" spans="2:23">
@@ -7301,7 +7130,7 @@
       <c r="S286" s="5"/>
       <c r="T286" s="5"/>
       <c r="U286" s="5"/>
-      <c r="V286" s="1"/>
+      <c r="V286" s="5"/>
       <c r="W286" s="7"/>
     </row>
     <row r="287" spans="2:23">
@@ -7323,7 +7152,7 @@
       <c r="S287" s="5"/>
       <c r="T287" s="5"/>
       <c r="U287" s="5"/>
-      <c r="V287" s="1"/>
+      <c r="V287" s="5"/>
       <c r="W287" s="7"/>
     </row>
     <row r="288" spans="2:23">
@@ -7345,7 +7174,7 @@
       <c r="S288" s="5"/>
       <c r="T288" s="5"/>
       <c r="U288" s="5"/>
-      <c r="V288" s="5"/>
+      <c r="V288" s="1"/>
       <c r="W288" s="7"/>
     </row>
     <row r="289" spans="2:23">
@@ -7367,7 +7196,7 @@
       <c r="S289" s="5"/>
       <c r="T289" s="5"/>
       <c r="U289" s="5"/>
-      <c r="V289" s="5"/>
+      <c r="V289" s="1"/>
       <c r="W289" s="7"/>
     </row>
     <row r="290" spans="2:23">
@@ -7389,7 +7218,7 @@
       <c r="S290" s="5"/>
       <c r="T290" s="5"/>
       <c r="U290" s="5"/>
-      <c r="V290" s="1"/>
+      <c r="V290" s="5"/>
       <c r="W290" s="7"/>
     </row>
     <row r="291" spans="2:23">
@@ -7433,7 +7262,7 @@
       <c r="S292" s="5"/>
       <c r="T292" s="5"/>
       <c r="U292" s="5"/>
-      <c r="V292" s="5"/>
+      <c r="V292" s="1"/>
       <c r="W292" s="7"/>
     </row>
     <row r="293" spans="2:23">
@@ -7961,7 +7790,7 @@
       <c r="S316" s="5"/>
       <c r="T316" s="5"/>
       <c r="U316" s="5"/>
-      <c r="V316" s="1"/>
+      <c r="V316" s="5"/>
       <c r="W316" s="7"/>
     </row>
     <row r="317" spans="2:23">
@@ -7983,7 +7812,7 @@
       <c r="S317" s="5"/>
       <c r="T317" s="5"/>
       <c r="U317" s="5"/>
-      <c r="V317" s="1"/>
+      <c r="V317" s="5"/>
       <c r="W317" s="7"/>
     </row>
     <row r="318" spans="2:23">
@@ -8071,7 +7900,7 @@
       <c r="S321" s="5"/>
       <c r="T321" s="5"/>
       <c r="U321" s="5"/>
-      <c r="V321" s="5"/>
+      <c r="V321" s="1"/>
       <c r="W321" s="7"/>
     </row>
     <row r="322" spans="2:23">
@@ -8093,7 +7922,7 @@
       <c r="S322" s="5"/>
       <c r="T322" s="5"/>
       <c r="U322" s="5"/>
-      <c r="V322" s="5"/>
+      <c r="V322" s="1"/>
       <c r="W322" s="7"/>
     </row>
     <row r="323" spans="2:23">
@@ -8159,7 +7988,7 @@
       <c r="S325" s="5"/>
       <c r="T325" s="5"/>
       <c r="U325" s="5"/>
-      <c r="V325" s="1"/>
+      <c r="V325" s="5"/>
       <c r="W325" s="7"/>
     </row>
     <row r="326" spans="2:23">
@@ -8181,7 +8010,7 @@
       <c r="S326" s="5"/>
       <c r="T326" s="5"/>
       <c r="U326" s="5"/>
-      <c r="V326" s="1"/>
+      <c r="V326" s="5"/>
       <c r="W326" s="7"/>
     </row>
     <row r="327" spans="2:23">
@@ -8203,7 +8032,7 @@
       <c r="S327" s="5"/>
       <c r="T327" s="5"/>
       <c r="U327" s="5"/>
-      <c r="V327" s="5"/>
+      <c r="V327" s="1"/>
       <c r="W327" s="7"/>
     </row>
     <row r="328" spans="2:23">
@@ -8225,7 +8054,7 @@
       <c r="S328" s="5"/>
       <c r="T328" s="5"/>
       <c r="U328" s="5"/>
-      <c r="V328" s="5"/>
+      <c r="V328" s="1"/>
       <c r="W328" s="7"/>
     </row>
     <row r="329" spans="2:23">
@@ -8247,7 +8076,7 @@
       <c r="S329" s="5"/>
       <c r="T329" s="5"/>
       <c r="U329" s="5"/>
-      <c r="V329" s="1"/>
+      <c r="V329" s="5"/>
       <c r="W329" s="7"/>
     </row>
     <row r="330" spans="2:23">
@@ -8269,7 +8098,7 @@
       <c r="S330" s="5"/>
       <c r="T330" s="5"/>
       <c r="U330" s="5"/>
-      <c r="V330" s="1"/>
+      <c r="V330" s="5"/>
       <c r="W330" s="7"/>
     </row>
     <row r="331" spans="2:23">
@@ -8291,7 +8120,7 @@
       <c r="S331" s="5"/>
       <c r="T331" s="5"/>
       <c r="U331" s="5"/>
-      <c r="V331" s="5"/>
+      <c r="V331" s="1"/>
       <c r="W331" s="7"/>
     </row>
     <row r="332" spans="2:23">
@@ -8313,7 +8142,7 @@
       <c r="S332" s="5"/>
       <c r="T332" s="5"/>
       <c r="U332" s="5"/>
-      <c r="V332" s="5"/>
+      <c r="V332" s="1"/>
       <c r="W332" s="7"/>
     </row>
     <row r="333" spans="2:23">
@@ -8643,7 +8472,7 @@
       <c r="S347" s="5"/>
       <c r="T347" s="5"/>
       <c r="U347" s="5"/>
-      <c r="V347" s="1"/>
+      <c r="V347" s="5"/>
       <c r="W347" s="7"/>
     </row>
     <row r="348" spans="2:23">
@@ -8665,7 +8494,7 @@
       <c r="S348" s="5"/>
       <c r="T348" s="5"/>
       <c r="U348" s="5"/>
-      <c r="V348" s="1"/>
+      <c r="V348" s="5"/>
       <c r="W348" s="7"/>
     </row>
     <row r="349" spans="2:23">
@@ -8687,7 +8516,7 @@
       <c r="S349" s="5"/>
       <c r="T349" s="5"/>
       <c r="U349" s="5"/>
-      <c r="V349" s="5"/>
+      <c r="V349" s="1"/>
       <c r="W349" s="7"/>
     </row>
     <row r="350" spans="2:23">
@@ -8709,7 +8538,7 @@
       <c r="S350" s="5"/>
       <c r="T350" s="5"/>
       <c r="U350" s="5"/>
-      <c r="V350" s="5"/>
+      <c r="V350" s="1"/>
       <c r="W350" s="7"/>
     </row>
     <row r="351" spans="2:23">
@@ -8819,7 +8648,7 @@
       <c r="S355" s="5"/>
       <c r="T355" s="5"/>
       <c r="U355" s="5"/>
-      <c r="V355" s="1"/>
+      <c r="V355" s="5"/>
       <c r="W355" s="7"/>
     </row>
     <row r="356" spans="2:23">
@@ -8841,7 +8670,7 @@
       <c r="S356" s="5"/>
       <c r="T356" s="5"/>
       <c r="U356" s="5"/>
-      <c r="V356" s="1"/>
+      <c r="V356" s="5"/>
       <c r="W356" s="7"/>
     </row>
     <row r="357" spans="2:23">
@@ -8863,7 +8692,7 @@
       <c r="S357" s="5"/>
       <c r="T357" s="5"/>
       <c r="U357" s="5"/>
-      <c r="V357" s="5"/>
+      <c r="V357" s="1"/>
       <c r="W357" s="7"/>
     </row>
     <row r="358" spans="2:23">
@@ -8885,7 +8714,7 @@
       <c r="S358" s="5"/>
       <c r="T358" s="5"/>
       <c r="U358" s="5"/>
-      <c r="V358" s="5"/>
+      <c r="V358" s="1"/>
       <c r="W358" s="7"/>
     </row>
     <row r="359" spans="2:23">
@@ -8907,7 +8736,7 @@
       <c r="S359" s="5"/>
       <c r="T359" s="5"/>
       <c r="U359" s="5"/>
-      <c r="V359" s="1"/>
+      <c r="V359" s="5"/>
       <c r="W359" s="7"/>
     </row>
     <row r="360" spans="2:23">
@@ -8951,7 +8780,7 @@
       <c r="S361" s="5"/>
       <c r="T361" s="5"/>
       <c r="U361" s="5"/>
-      <c r="V361" s="5"/>
+      <c r="V361" s="1"/>
       <c r="W361" s="7"/>
     </row>
     <row r="362" spans="2:23">
@@ -9391,7 +9220,7 @@
       <c r="S381" s="5"/>
       <c r="T381" s="5"/>
       <c r="U381" s="5"/>
-      <c r="V381" s="1"/>
+      <c r="V381" s="5"/>
       <c r="W381" s="7"/>
     </row>
     <row r="382" spans="2:23">
@@ -9413,7 +9242,7 @@
       <c r="S382" s="5"/>
       <c r="T382" s="5"/>
       <c r="U382" s="5"/>
-      <c r="V382" s="1"/>
+      <c r="V382" s="5"/>
       <c r="W382" s="7"/>
     </row>
     <row r="383" spans="2:23">
@@ -9501,7 +9330,7 @@
       <c r="S386" s="5"/>
       <c r="T386" s="5"/>
       <c r="U386" s="5"/>
-      <c r="V386" s="5"/>
+      <c r="V386" s="1"/>
       <c r="W386" s="7"/>
     </row>
     <row r="387" spans="2:23">
@@ -9523,7 +9352,7 @@
       <c r="S387" s="5"/>
       <c r="T387" s="5"/>
       <c r="U387" s="5"/>
-      <c r="V387" s="5"/>
+      <c r="V387" s="1"/>
       <c r="W387" s="7"/>
     </row>
     <row r="388" spans="2:23">
@@ -9589,7 +9418,7 @@
       <c r="S390" s="5"/>
       <c r="T390" s="5"/>
       <c r="U390" s="5"/>
-      <c r="V390" s="1"/>
+      <c r="V390" s="5"/>
       <c r="W390" s="7"/>
     </row>
     <row r="391" spans="2:23">
@@ -9611,7 +9440,7 @@
       <c r="S391" s="5"/>
       <c r="T391" s="5"/>
       <c r="U391" s="5"/>
-      <c r="V391" s="1"/>
+      <c r="V391" s="5"/>
       <c r="W391" s="7"/>
     </row>
     <row r="392" spans="2:23">
@@ -9633,7 +9462,7 @@
       <c r="S392" s="5"/>
       <c r="T392" s="5"/>
       <c r="U392" s="5"/>
-      <c r="V392" s="5"/>
+      <c r="V392" s="1"/>
       <c r="W392" s="7"/>
     </row>
     <row r="393" spans="2:23">
@@ -9655,7 +9484,7 @@
       <c r="S393" s="5"/>
       <c r="T393" s="5"/>
       <c r="U393" s="5"/>
-      <c r="V393" s="5"/>
+      <c r="V393" s="1"/>
       <c r="W393" s="7"/>
     </row>
     <row r="394" spans="2:23">
@@ -9677,7 +9506,7 @@
       <c r="S394" s="5"/>
       <c r="T394" s="5"/>
       <c r="U394" s="5"/>
-      <c r="V394" s="1"/>
+      <c r="V394" s="5"/>
       <c r="W394" s="7"/>
     </row>
     <row r="395" spans="2:23">
@@ -9699,7 +9528,7 @@
       <c r="S395" s="5"/>
       <c r="T395" s="5"/>
       <c r="U395" s="5"/>
-      <c r="V395" s="1"/>
+      <c r="V395" s="5"/>
       <c r="W395" s="7"/>
     </row>
     <row r="396" spans="2:23">
@@ -9721,7 +9550,7 @@
       <c r="S396" s="5"/>
       <c r="T396" s="5"/>
       <c r="U396" s="5"/>
-      <c r="V396" s="5"/>
+      <c r="V396" s="1"/>
       <c r="W396" s="7"/>
     </row>
     <row r="397" spans="2:23">
@@ -9743,7 +9572,7 @@
       <c r="S397" s="5"/>
       <c r="T397" s="5"/>
       <c r="U397" s="5"/>
-      <c r="V397" s="5"/>
+      <c r="V397" s="1"/>
       <c r="W397" s="7"/>
     </row>
     <row r="398" spans="2:23">
@@ -9989,7 +9818,6 @@
       <c r="W408" s="7"/>
     </row>
     <row r="409" spans="1:23">
-      <c r="A409" s="8"/>
       <c r="B409" s="5"/>
       <c r="C409" s="5"/>
       <c r="D409" s="5"/>
@@ -10034,6 +9862,7 @@
       <c r="W410" s="7"/>
     </row>
     <row r="411" spans="1:23">
+      <c r="A411" s="8"/>
       <c r="B411" s="5"/>
       <c r="C411" s="5"/>
       <c r="D411" s="5"/>
@@ -10074,7 +9903,7 @@
       <c r="S412" s="5"/>
       <c r="T412" s="5"/>
       <c r="U412" s="5"/>
-      <c r="V412" s="1"/>
+      <c r="V412" s="5"/>
       <c r="W412" s="7"/>
     </row>
     <row r="413" spans="1:23">
@@ -10096,7 +9925,7 @@
       <c r="S413" s="5"/>
       <c r="T413" s="5"/>
       <c r="U413" s="5"/>
-      <c r="V413" s="1"/>
+      <c r="V413" s="5"/>
       <c r="W413" s="7"/>
     </row>
     <row r="414" spans="1:23">
@@ -10118,7 +9947,7 @@
       <c r="S414" s="5"/>
       <c r="T414" s="5"/>
       <c r="U414" s="5"/>
-      <c r="V414" s="5"/>
+      <c r="V414" s="1"/>
       <c r="W414" s="7"/>
     </row>
     <row r="415" spans="1:23">
@@ -10140,11 +9969,10 @@
       <c r="S415" s="5"/>
       <c r="T415" s="5"/>
       <c r="U415" s="5"/>
-      <c r="V415" s="5"/>
+      <c r="V415" s="1"/>
       <c r="W415" s="7"/>
     </row>
     <row r="416" spans="1:23">
-      <c r="A416" s="3"/>
       <c r="B416" s="5"/>
       <c r="C416" s="5"/>
       <c r="D416" s="5"/>
@@ -10167,7 +9995,6 @@
       <c r="W416" s="7"/>
     </row>
     <row r="417" spans="1:23">
-      <c r="A417" s="8"/>
       <c r="B417" s="5"/>
       <c r="C417" s="5"/>
       <c r="D417" s="5"/>
@@ -10190,6 +10017,7 @@
       <c r="W417" s="7"/>
     </row>
     <row r="418" spans="1:23">
+      <c r="A418" s="3"/>
       <c r="B418" s="5"/>
       <c r="C418" s="5"/>
       <c r="D418" s="5"/>
@@ -10212,6 +10040,7 @@
       <c r="W418" s="7"/>
     </row>
     <row r="419" spans="1:23">
+      <c r="A419" s="8"/>
       <c r="B419" s="5"/>
       <c r="C419" s="5"/>
       <c r="D419" s="5"/>
@@ -10252,7 +10081,7 @@
       <c r="S420" s="5"/>
       <c r="T420" s="5"/>
       <c r="U420" s="5"/>
-      <c r="V420" s="1"/>
+      <c r="V420" s="5"/>
       <c r="W420" s="7"/>
     </row>
     <row r="421" spans="1:23">
@@ -10274,7 +10103,7 @@
       <c r="S421" s="5"/>
       <c r="T421" s="5"/>
       <c r="U421" s="5"/>
-      <c r="V421" s="1"/>
+      <c r="V421" s="5"/>
       <c r="W421" s="7"/>
     </row>
     <row r="422" spans="1:23">
@@ -10296,7 +10125,7 @@
       <c r="S422" s="5"/>
       <c r="T422" s="5"/>
       <c r="U422" s="5"/>
-      <c r="V422" s="5"/>
+      <c r="V422" s="1"/>
       <c r="W422" s="7"/>
     </row>
     <row r="423" spans="1:23">
@@ -10318,7 +10147,7 @@
       <c r="S423" s="5"/>
       <c r="T423" s="5"/>
       <c r="U423" s="5"/>
-      <c r="V423" s="5"/>
+      <c r="V423" s="1"/>
       <c r="W423" s="7"/>
     </row>
     <row r="424" spans="1:23">
@@ -10340,8 +10169,52 @@
       <c r="S424" s="5"/>
       <c r="T424" s="5"/>
       <c r="U424" s="5"/>
-      <c r="V424" s="1"/>
+      <c r="V424" s="5"/>
       <c r="W424" s="7"/>
+    </row>
+    <row r="425" spans="1:23">
+      <c r="B425" s="5"/>
+      <c r="C425" s="5"/>
+      <c r="D425" s="5"/>
+      <c r="E425" s="5"/>
+      <c r="H425" s="5"/>
+      <c r="I425" s="5"/>
+      <c r="J425" s="5"/>
+      <c r="K425" s="5"/>
+      <c r="L425" s="5"/>
+      <c r="M425" s="6"/>
+      <c r="N425" s="5"/>
+      <c r="O425" s="5"/>
+      <c r="P425" s="5"/>
+      <c r="Q425" s="5"/>
+      <c r="R425" s="5"/>
+      <c r="S425" s="5"/>
+      <c r="T425" s="5"/>
+      <c r="U425" s="5"/>
+      <c r="V425" s="5"/>
+      <c r="W425" s="7"/>
+    </row>
+    <row r="426" spans="1:23">
+      <c r="B426" s="5"/>
+      <c r="C426" s="5"/>
+      <c r="D426" s="5"/>
+      <c r="E426" s="5"/>
+      <c r="H426" s="5"/>
+      <c r="I426" s="5"/>
+      <c r="J426" s="5"/>
+      <c r="K426" s="5"/>
+      <c r="L426" s="5"/>
+      <c r="M426" s="6"/>
+      <c r="N426" s="5"/>
+      <c r="O426" s="5"/>
+      <c r="P426" s="5"/>
+      <c r="Q426" s="5"/>
+      <c r="R426" s="5"/>
+      <c r="S426" s="5"/>
+      <c r="T426" s="5"/>
+      <c r="U426" s="5"/>
+      <c r="V426" s="1"/>
+      <c r="W426" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>